<commit_message>
Enhance bouquet management: add handling for empty bouquets, improve bouquet loading logic, and update UI tab refresh for order and quantities
</commit_message>
<xml_diff>
--- a/Bouquets.xlsx
+++ b/Bouquets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>אלסטרומריה</t>
+          <t>בוקט ורדים גדול (based on ורד אדום קטן)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>אלסטרומריה</t>
+          <t>גפסנית</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>בוקט פרחי חורף</t>
+          <t>בוקט ורדים גדול (based on ורד אדום קטן)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>נוריות</t>
+          <t>ורד</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>צבעוני</t>
+          <t>אדום</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>רגיל</t>
+          <t>גדול</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -513,82 +513,82 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>בוקט פרחי חורף</t>
+          <t>ורד אדום קטן</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>כלניות</t>
+          <t>ורד</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>צבעוני</t>
+          <t>אדום</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>רגיל</t>
+          <t>קטן</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>בוקט פרחי חורף</t>
+          <t>ורד אדום קטן</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>גרברה</t>
+          <t>גפסנית</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>צבעוני</t>
+          <t>לבן</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>קטן</t>
+          <t>רגיל</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>בוקט פרחי חורף</t>
+          <t>ורד ענק</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>אקליפטוס</t>
+          <t>ורד</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>צבעוני</t>
+          <t>אדום</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>רגיל</t>
+          <t>קטן</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>בוקט פרחי חורף</t>
+          <t>ורד ענק</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -607,82 +607,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>בוקט פרחי חורף</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>שעווה</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>צבעוני</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>רגיל</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>צבעוני אדום</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>צבעוני</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>אדום</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>רגיל</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>צבעוני בהפתעה (based on צבעוני אדום)</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>צבעוני</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>אדום</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>רגיל</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>